<commit_message>
feat: add robot to the project
</commit_message>
<xml_diff>
--- a/Doc/Upload.xlsx
+++ b/Doc/Upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\Szakdolgozat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F96B8DB-620A-4FAC-8A76-0A09C1F52F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CBC84E-ABB6-44CB-AB99-81F5BA056146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Monitor</t>
   </si>
@@ -98,10 +98,22 @@
     <t>Currys</t>
   </si>
   <si>
-    <t>Curryes.co.uk</t>
-  </si>
-  <si>
     <t>BlueRay</t>
+  </si>
+  <si>
+    <t>https://www.currys.co.uk/</t>
+  </si>
+  <si>
+    <t>https://www.hobbycraft.co.uk/</t>
+  </si>
+  <si>
+    <t>hobbycraft</t>
+  </si>
+  <si>
+    <t>hm.com</t>
+  </si>
+  <si>
+    <t>hm</t>
   </si>
 </sst>
 </file>
@@ -137,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -516,7 +529,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -569,16 +582,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -612,7 +625,23 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc: update upload file
</commit_message>
<xml_diff>
--- a/Doc/Upload.xlsx
+++ b/Doc/Upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CBC84E-ABB6-44CB-AB99-81F5BA056146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF57B6C6-0112-40AD-87ED-DE8CCC2A4003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="2" r:id="rId1"/>
@@ -27,50 +27,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Monitor</t>
   </si>
   <si>
-    <t>Memory</t>
-  </si>
-  <si>
-    <t>HDD</t>
-  </si>
-  <si>
-    <t>CPU</t>
-  </si>
-  <si>
     <t>CategoryName</t>
   </si>
   <si>
     <t>ComputerPartName</t>
   </si>
   <si>
-    <t>LCD</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>OLED</t>
-  </si>
-  <si>
-    <t>DDR4</t>
-  </si>
-  <si>
-    <t>DDR3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SODIMM </t>
-  </si>
-  <si>
-    <t>3.5-inch Internal Hard Drive</t>
-  </si>
-  <si>
-    <t>Intel Core i7 Processor</t>
-  </si>
-  <si>
     <t>WebshopName</t>
   </si>
   <si>
@@ -89,18 +56,12 @@
     <t>Ebay.com</t>
   </si>
   <si>
-    <t>DVD Reader</t>
-  </si>
-  <si>
     <t>DVD</t>
   </si>
   <si>
     <t>Currys</t>
   </si>
   <si>
-    <t>BlueRay</t>
-  </si>
-  <si>
     <t>https://www.currys.co.uk/</t>
   </si>
   <si>
@@ -114,6 +75,54 @@
   </si>
   <si>
     <t>hm</t>
+  </si>
+  <si>
+    <t>Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory </t>
+  </si>
+  <si>
+    <t>Power Supplie</t>
+  </si>
+  <si>
+    <t>Computer Case</t>
+  </si>
+  <si>
+    <t>Graphics Card</t>
+  </si>
+  <si>
+    <t>Network Card</t>
+  </si>
+  <si>
+    <t>Processors</t>
+  </si>
+  <si>
+    <t>Sound Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard drive </t>
+  </si>
+  <si>
+    <t>24 Inch Full HD Monitor</t>
+  </si>
+  <si>
+    <t>1TB HDD</t>
+  </si>
+  <si>
+    <t>Intel Core i5</t>
+  </si>
+  <si>
+    <t>motherboard atx DDR4</t>
+  </si>
+  <si>
+    <t>ddr4 64GB</t>
+  </si>
+  <si>
+    <t>ATX Mid Tower Gaming Case</t>
+  </si>
+  <si>
+    <t>AMD Radeon RX</t>
   </si>
 </sst>
 </file>
@@ -149,9 +158,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,15 +454,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -462,74 +470,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -539,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FF62CF-2793-4A0D-9ED0-43745A45E840}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +536,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -562,17 +546,52 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -598,50 +617,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -650,14 +669,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -903,21 +920,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -943,9 +959,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(robot): Add try-catch blocks to handle exceptions
</commit_message>
<xml_diff>
--- a/Doc/Upload.xlsx
+++ b/Doc/Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF57B6C6-0112-40AD-87ED-DE8CCC2A4003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83DD2A6-4213-4567-BE69-1F17B83A13C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Monitor</t>
   </si>
@@ -56,27 +56,12 @@
     <t>Ebay.com</t>
   </si>
   <si>
-    <t>DVD</t>
-  </si>
-  <si>
     <t>Currys</t>
   </si>
   <si>
     <t>https://www.currys.co.uk/</t>
   </si>
   <si>
-    <t>https://www.hobbycraft.co.uk/</t>
-  </si>
-  <si>
-    <t>hobbycraft</t>
-  </si>
-  <si>
-    <t>hm.com</t>
-  </si>
-  <si>
-    <t>hm</t>
-  </si>
-  <si>
     <t>Motherboard</t>
   </si>
   <si>
@@ -95,34 +80,31 @@
     <t>Network Card</t>
   </si>
   <si>
-    <t>Processors</t>
-  </si>
-  <si>
     <t>Sound Card</t>
   </si>
   <si>
     <t xml:space="preserve">hard drive </t>
   </si>
   <si>
-    <t>24 Inch Full HD Monitor</t>
-  </si>
-  <si>
     <t>1TB HDD</t>
   </si>
   <si>
-    <t>Intel Core i5</t>
-  </si>
-  <si>
-    <t>motherboard atx DDR4</t>
-  </si>
-  <si>
-    <t>ddr4 64GB</t>
-  </si>
-  <si>
     <t>ATX Mid Tower Gaming Case</t>
   </si>
   <si>
-    <t>AMD Radeon RX</t>
+    <t>AMD Ryzen 5 7600X</t>
+  </si>
+  <si>
+    <t>32GB DDR5 5600MHz</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 4060</t>
+  </si>
+  <si>
+    <t>Gigabyte B650 AORUS ELITE AX AMD B650 Chipset</t>
+  </si>
+  <si>
+    <t>Processor</t>
   </si>
 </sst>
 </file>
@@ -158,8 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -462,58 +447,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
+      <c r="A3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -523,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FF62CF-2793-4A0D-9ED0-43745A45E840}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,52 +523,47 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -601,10 +573,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,26 +613,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(robot): add price parser custom activity
</commit_message>
<xml_diff>
--- a/Doc/Upload.xlsx
+++ b/Doc/Upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83DD2A6-4213-4567-BE69-1F17B83A13C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB25ED3-ABF6-41CA-A8D9-781B78383B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Monitor</t>
   </si>
@@ -44,24 +44,6 @@
     <t>WebshopURL</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>EBAY</t>
-  </si>
-  <si>
-    <t>Amazon.com</t>
-  </si>
-  <si>
-    <t>Ebay.com</t>
-  </si>
-  <si>
-    <t>Currys</t>
-  </si>
-  <si>
-    <t>https://www.currys.co.uk/</t>
-  </si>
-  <si>
     <t>Motherboard</t>
   </si>
   <si>
@@ -89,32 +71,61 @@
     <t>1TB HDD</t>
   </si>
   <si>
-    <t>ATX Mid Tower Gaming Case</t>
+    <t>32GB DDR5 5600MHz</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>GeForce RTX 4060</t>
+  </si>
+  <si>
+    <t>B650 AORUS ELITE AX AMD B650</t>
+  </si>
+  <si>
+    <t>Emag</t>
+  </si>
+  <si>
+    <t>http://emag.hu</t>
+  </si>
+  <si>
+    <t>Alza</t>
+  </si>
+  <si>
+    <t>http://alza.hu</t>
+  </si>
+  <si>
+    <t>Pcx</t>
+  </si>
+  <si>
+    <t>http://pcx.hu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard drive </t>
   </si>
   <si>
     <t>AMD Ryzen 5 7600X</t>
   </si>
   <si>
-    <t>32GB DDR5 5600MHz</t>
-  </si>
-  <si>
-    <t>NVIDIA GeForce RTX 4060</t>
-  </si>
-  <si>
-    <t>Gigabyte B650 AORUS ELITE AX AMD B650 Chipset</t>
-  </si>
-  <si>
-    <t>Processor</t>
+    <t>ATX Tower Gaming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,16 +148,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,7 +442,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,50 +461,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +517,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,47 +537,47 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +590,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,40 +611,47 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DC05E364-51B2-40C0-AACC-ACBCA3D93755}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9481404B-28C8-44BE-A270-A6F878179DFD}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{BBB29A76-B2A2-4FA6-822A-36E035B4664A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -876,20 +897,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -915,12 +937,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(szakdolgozat): extend documentation with Teljesítmény
</commit_message>
<xml_diff>
--- a/Doc/Upload.xlsx
+++ b/Doc/Upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB25ED3-ABF6-41CA-A8D9-781B78383B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E1FB6F-8F51-40D5-9F3E-9EBD182A9575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Monitor</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>ATX Tower Gaming</t>
+  </si>
+  <si>
+    <t>https://www.bestbyte.hu</t>
+  </si>
+  <si>
+    <t>Bestbyte</t>
   </si>
 </sst>
 </file>
@@ -441,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,10 +593,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,25 +639,32 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DC05E364-51B2-40C0-AACC-ACBCA3D93755}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{9481404B-28C8-44BE-A270-A6F878179DFD}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{BBB29A76-B2A2-4FA6-822A-36E035B4664A}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{93028E98-6F6E-4955-ACB4-DF0873BF697F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -897,21 +910,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -937,9 +949,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>